<commit_message>
Modify the part of initialization in window_oneSol_dp_v2() and reduced_dp(), and delete redundant code
</commit_message>
<xml_diff>
--- a/C++/result_density.xlsx
+++ b/C++/result_density.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ncku365-my.sharepoint.com/personal/f74056124_ncku_edu_tw/Documents/Lab/Lane-Merging/C++/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{5C46E978-0C45-4498-80D4-7F54B41DA6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95707A90-0F7B-4A7A-9100-B28D92F2FB90}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{5C46E978-0C45-4498-80D4-7F54B41DA6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{346C5410-7C7D-43A5-8DBE-95E98642E3E0}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="8964" xr2:uid="{36926230-96B8-4722-A7EB-88AD92889262}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36926230-96B8-4722-A7EB-88AD92889262}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00988A3-4749-4401-AC27-E9A173322710}">
   <dimension ref="A1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13:AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -6149,24 +6149,27 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="A15:AD15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="S58:U58"/>
+    <mergeCell ref="V58:X58"/>
+    <mergeCell ref="Y58:AA58"/>
+    <mergeCell ref="AB58:AD58"/>
+    <mergeCell ref="S44:U44"/>
+    <mergeCell ref="V44:X44"/>
+    <mergeCell ref="Y44:AA44"/>
+    <mergeCell ref="AB44:AD44"/>
+    <mergeCell ref="A57:AD57"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="J58:L58"/>
+    <mergeCell ref="M58:O58"/>
     <mergeCell ref="A43:AD43"/>
     <mergeCell ref="S16:U16"/>
     <mergeCell ref="V16:X16"/>
@@ -6183,27 +6186,24 @@
     <mergeCell ref="V30:X30"/>
     <mergeCell ref="Y30:AA30"/>
     <mergeCell ref="AB30:AD30"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="J58:L58"/>
-    <mergeCell ref="M58:O58"/>
-    <mergeCell ref="S44:U44"/>
-    <mergeCell ref="V44:X44"/>
-    <mergeCell ref="Y44:AA44"/>
-    <mergeCell ref="AB44:AD44"/>
-    <mergeCell ref="A57:AD57"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="S58:U58"/>
-    <mergeCell ref="V58:X58"/>
-    <mergeCell ref="Y58:AA58"/>
-    <mergeCell ref="AB58:AD58"/>
+    <mergeCell ref="A15:AD15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>